<commit_message>
Documentaion update 16 May 2018
</commit_message>
<xml_diff>
--- a/docs/_static/xlsx/tab_Stato_civile.xlsx
+++ b/docs/_static/xlsx/tab_Stato_civile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t/>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Unito civilmente</t>
+  </si>
+  <si>
+    <t>Stato libero a seguito di scioglimento dell'unione</t>
+  </si>
+  <si>
+    <t>Stato libero a seguito di decesso della parte unita civilmente</t>
   </si>
 </sst>
 </file>
@@ -397,11 +403,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -490,6 +496,28 @@
       </c>
       <c r="C7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -627,13 +655,40 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D712B8-3498-4CB5-9601-ED2BF20F84B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D712B8-3498-4CB5-9601-ED2BF20F84B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E98BBD55-B719-46BF-97B4-739F6451CC39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E98BBD55-B719-46BF-97B4-739F6451CC39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E1B371B-19ED-4FCA-828C-FFB43B6ADADF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E1B371B-19ED-4FCA-828C-FFB43B6ADADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>